<commit_message>
Update van de API-testing en het Testplan Spring 1.
</commit_message>
<xml_diff>
--- a/Sprint 1/Testplan Mutualism Sprint 1.xlsx
+++ b/Sprint 1/Testplan Mutualism Sprint 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12103550\Desktop\3TIN\IT-project\Testing\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12103550\Desktop\3TIN\IT-project\Testing\GitHubRepo\Mutualism-Testing\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D16613F-4AEE-46D1-B51F-95DE4B152592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8472DC71-EA4E-4016-95C1-BB7D694A2931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7518049B-637E-4A85-8860-D7600403E9F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="79">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -359,6 +359,92 @@
     <t>Open mobiele applicatie.
 Klik op map-button.
 Beoordeel aanwezigheid lijst-button op 'Tree List'-scherm.</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>Test op login-API waarmee een gebruiker niet kan inloggen zonder account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Login met onbestaande gebruiker.</t>
+  </si>
+  <si>
+    <t>Username: "wronguser"
+Password: "wrongwachtwoord"</t>
+  </si>
+  <si>
+    <t>Login
+Statuscode: 200
+Response time &lt; 500
+access_token: not empty
+token_type = bearer</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>Registreer nieuwe gebruiker met random password
+Login met nieuwe gebruiker en fout password</t>
+  </si>
+  <si>
+    <t>Username: random via faker library
+Password: "wrongpassword"</t>
+  </si>
+  <si>
+    <t>Registratie
+Statuscode: 200
+Response time &lt; 500
+Response = complete
+Login
+Statuscode: 401
+Response time &lt; 500
+access_token: not empty
+token_type = bearer</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>Test op login via webinterface met bestaande account.</t>
+  </si>
+  <si>
+    <t>Login met bestaande gebruiker</t>
+  </si>
+  <si>
+    <t>Username: "testuser"
+Password: "testpassword"</t>
+  </si>
+  <si>
+    <t>Ingelogd als bestaande gebruiker.</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>Test op logout via webinterface met bestaande account.</t>
+  </si>
+  <si>
+    <t>Login met bestaande gebruiker
+Logout met bestaande gebruiker</t>
+  </si>
+  <si>
+    <t>Ingelogd als bestaande gebruiker.
+Uitgelogd als bestaande gebruiker.</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>Test op login via webinterface met niet-bestaande account.</t>
+  </si>
+  <si>
+    <t>Login met niet-bestaande gebruiker</t>
+  </si>
+  <si>
+    <t>Niet ingelogd. 
+ErrorMessage: "Ongeldige gebruikersnaam of wachtwoord."</t>
   </si>
 </sst>
 </file>
@@ -779,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E01415B-97DC-4DD5-ACA3-9D5479E376E6}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1158,121 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>